<commit_message>
Updated User Stories and Scrum Role
</commit_message>
<xml_diff>
--- a/Agile-ASSIGNMENT.xlsx
+++ b/Agile-ASSIGNMENT.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24923"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tcsdatacifs09.corp.trizetto.com\citrixprofiles\sandya.shanmugham.upm\DATA\Documents\Agile Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BITS_Agile_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="11_A1BEBF06E04E374AA84E82C3CB33F32C5865AB09" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF6C2C93-4664-495B-9715-C9B9246500E6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Evalution citeria " sheetId="1" r:id="rId1"/>
     <sheet name="Case Study 1  Facify-me" sheetId="2" r:id="rId2"/>
     <sheet name="Case Study 1 - User Stories" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t xml:space="preserve">Assignment evalution citeria </t>
   </si>
@@ -219,76 +218,33 @@
 i) Navigation bar with necessary details.</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1) Create homepage for facify-me app which will have  navigation bar with required tabs/dropdowns.
-Description – 
-facify-me homepage navigation bar should contain the following  tabs/dropdowns :                                                                                      i) It should contain About us dropdown which will have   contact us/team wins/ our achievements option
-ii) login/logout tab.
-</t>
-  </si>
-  <si>
     <t>Acceptance Criteria – Homepage created with the navigation bar containg the required tabs/dropdown.</t>
   </si>
   <si>
     <t>ii) Dashboard summary no of games, teams wins, next match, Team details, Available slots for ground</t>
   </si>
   <si>
-    <t>1.2) Create GUI frame for homepage of facify-me app with the necessary dashboard contents.
-Description – 
-facify-me homepage should contain the different cards with following contents :                                                                                      i) Display the Dashboard summary.
-ii) Team Details/Team wins.                                                                                 iii) Number of matches organized by facify-me.                                    iv) Total count of countries where we organize the event.                  v)   Ground Details - It will contain available slots.</t>
-  </si>
-  <si>
-    <t>All required cards are successfully created and displayed in dashboard.</t>
-  </si>
-  <si>
     <t>iii) Backend functionaliy.</t>
   </si>
   <si>
     <t>1.3) Implement backend functionaliy(only for next available slots of ground) using get method to fetch the details from required table based on the differnt card contents.</t>
   </si>
   <si>
-    <t>Succesfully able to display the next available ground details.</t>
-  </si>
-  <si>
     <t>2. Registration Module</t>
   </si>
   <si>
     <t>Registration page will be accessed by Admin only. Admin will have the access to register the members.</t>
   </si>
   <si>
-    <t xml:space="preserve">2.1)	Create Registration webpage for each Member with their access_groups name and only general admin can access this page to add the other members details.
-i)	Input fields – Member_Name, Age, DOB, Gender,                              Access_group, Country, Contact_No, Email_Id,                
-Password, Confirm_Password.                                                            If access_group name is Player/Coach then one extra input field is mandatory i.e. Team_Name.                        
-ii)	Button –  Create Register Button at bottom of registration page. 
-</t>
-  </si>
-  <si>
     <t>Acceptance Criteria – Registration Page created with required input fields and validations.</t>
   </si>
   <si>
     <t>Perform the required validations on input field. All the fields are mandatory except team_name which is only mandatory where access_group is player/coach.</t>
   </si>
   <si>
-    <t xml:space="preserve">2.2) Registration page input field should have proper input validations.                                                                                                i) All fields are mandatory.                                                                  ii) DOB – YYYY/MM/DD
-iii) Email – abc@xyz.com
-iv) Password – a) Maximum 7 characters.
-		       	   b) both cases should be present with at least one special characters and digit.                                                                            
-v) Confirm Password - It should match with the password   field value.          
-vi) If access_group is player/coach then team_name field is mandatory.                                                                                                                           vii) Button should be enable only when all fields are successfully validated.                                                                   </t>
-  </si>
-  <si>
     <t>Acceptance Criteria – Input fields validated for registration page.</t>
   </si>
   <si>
-    <t xml:space="preserve">2.3) Create table for member details in database.
-i)Table Name:  member_details.
-Column names:                                                                                              i) user_name – varchar(2) – Len60 
-ii) gender – varchar(2) – Len60                                                                                                                                                                                                                                                   iii) age – number                                                                                                                                                 
-iv) password - varchar(2) – Len60 (should be in encrypted form)
-v) access_group – varchar                                                                            vi) email_id - varchar                                                                                         vii) contact - number                                                                                                          viii) team_name - varchar (only for users where access_group field is player/coach).
-</t>
-  </si>
-  <si>
     <t>Acceptance Criteria – New table created with required columns for team details.</t>
   </si>
   <si>
@@ -298,9 +254,6 @@
     <t>2.4) Create backend logic and implement post method to send the regisration details to backend table.</t>
   </si>
   <si>
-    <t>User successfully able o register and the user details are successfully inserted into the table.</t>
-  </si>
-  <si>
     <t>3. Login Page</t>
   </si>
   <si>
@@ -308,9 +261,6 @@
   </si>
   <si>
     <t>3.1) Create login page with two input fields userid and password. Login button will enable only when both userid and password is submitted.                                                                                                           3.2) Create backend logic to implement any secure login technology(example JWT) .                                                                              3.3) Create forgot password page where user need to give user id, old password , new password and confirm new password and click on the submit button.                                                                                                  3.4) After clicking on the submit button password needs to be updated in the table.</t>
-  </si>
-  <si>
-    <t>Successfully able to login or reset the password.</t>
   </si>
   <si>
     <t xml:space="preserve">4. Content Editor page </t>
@@ -324,9 +274,6 @@
 4.3 Ensure there will be only 4 slots will present per ground business logic </t>
   </si>
   <si>
-    <t>Admin successfully able update the content  and the match details  are successfully inserted/updated  into the table.</t>
-  </si>
-  <si>
     <t>5. Ground Details</t>
   </si>
   <si>
@@ -336,38 +283,117 @@
     <t>5.1 Create a form to insert the ground details and make ensure there will be maximum four slots will be present and this form should have submit button which will be enable only after all mandatory details will be populated successfully and make sure this page will be only accessible by admin.                                                  5.2 Create a table in db which will store all ground related details.           5.3 Create business logic for validation and insert/update the data into the db.</t>
   </si>
   <si>
-    <t>Successfully inserted the data of ground details in db by admin.</t>
-  </si>
-  <si>
     <t>6. Booking Ground</t>
   </si>
   <si>
     <t>Ground details will be shown in form of grid with the book/Cancel button for each ground details.</t>
   </si>
   <si>
-    <t>6.1 Create a web page for showing the ground details such as ground name, ground location, ground status(available/booked/waiting for approval), team name if a ground is booked and .                                                                             6.2 Create booking/Cancel button that will be only visible to access_groupis admin.                                                                                      6.3 Create a business logic to fetch/update the details from/to the DB and trigger the mail to 5 executives.</t>
-  </si>
-  <si>
-    <t>Admin successfully able to send booking/cancel requests of ground and all relevant ground details are displayed in the ground availability page. Successfully mail will be trigerred after clicking on booking/cancel button.</t>
-  </si>
-  <si>
     <t>7. SMS functionality</t>
   </si>
   <si>
-    <t>Create business logic so that after booking/cancelling/change in slot sms will be sent to the respective person.</t>
-  </si>
-  <si>
     <t>Create business logic to check the approval count of executives if it is equal to 2 then approved sms/mail will be sent to the team members/coach.</t>
   </si>
   <si>
-    <t>SMS/Mail successfully sent after approval of two executive.</t>
+    <t xml:space="preserve">2.1)	Create Registration webpage for each Member with their access_groups name and only general admin can access this page to add the other members details.
+i)	Input fields – Member_Name, Age, DOB, Gender,                              Access_group, Country, Contact_No, Email_Id,                
+Password, Confirm_Password.                                                                        If access_group name is Player/Coach then one extra input field is mandatory i.e. Team_Name.                        
+ii)	Button –  Create Register Button at bottom of registration page. 
+</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria- Succesfully able to display the next available ground details.</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria- User successfully able o register and the user details are successfully inserted into the table.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3) Create table for member details in database.
+i)Table Name:  member_details.
+Column names:                                                                                                     i) user_name – varchar(2) – Len60 
+ii) gender – varchar(2) – Len60                                                                                                                                                                                                                                                   iii) age – number                                                                                                                                                 
+iv) password - varchar(2) – Len60 (should be in encrypted form)
+v) access_group – varchar                                                                               vi) email_id - varchar                                                                                         vii) contact - number                                                                                                          viii) team_name - varchar (only for users where access_group field is player/coach).
+</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria- Successfully able to login or reset the password.</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria- Admin successfully able update the content  and the match details  are successfully inserted/updated  into the table.</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria- Successfully inserted the data of ground details in db by admin.</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria- Admin successfully able to send booking/cancel requests of ground and all relevant ground details are displayed in the ground availability page. Successfully mail will be trigerred after clicking on booking/cancel button.</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria- SMS/Mail successfully sent after approval of two executive.</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - All required cards are successfully created and displayed in dashboard.</t>
+  </si>
+  <si>
+    <t>1.2) Create GUI frame for homepage of facify-me app with the necessary dashboard contents.
+Description – 
+facify-me homepage should contain the different cards with following contents :                                                                                            i) Display the Dashboard summary.
+ii) Team Details/Team wins.                                                                                 iii) Number of matches organized by facify-me.                                    iv) Total count of countries where we organize the event.                  v)   Ground Details - It will contain available slots.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1) Create homepage for facify-me app which will have  navigation bar with required tabs/dropdowns.
+Description – 
+facify-me homepage navigation bar should contain the following  tabs/dropdowns :                                                                                                  i) It should contain About us dropdown which will have   contact us/team wins/ our achievements option
+ii) login/logout tab.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2) Registration page input field should have proper input validations.                                                                                                             i) All fields are mandatory.                                                                             ii) DOB – YYYY/MM/DD
+iii) Email – abc@xyz.com
+iv) Password – a) Maximum 7 characters.
+		                      	   b) both cases should be present with at least one special characters and digit.                                                                            
+v) Confirm Password - It should match with the password   field value.          
+vi) If access_group is player/coach then team_name field is mandatory.                                                                                                                           vii) Button should be enable only when all fields are successfully validated.                                                                   </t>
+  </si>
+  <si>
+    <t>6.1 Create a web page for showing the ground details such as ground name, ground location, ground status(available/booked/waiting for approval), team name if a ground is booked and .                                                                                     6.2 Create booking/Cancel button that will be only visible to access_groupis admin.                                                                                      6.3 Create a business logic to fetch/update the details from/to the DB and trigger the mail to 5 executives.</t>
+  </si>
+  <si>
+    <t>8. Change Request</t>
+  </si>
+  <si>
+    <t>Create Web Page to show the booked ground details to coach so, that he can raise the request for changing the slot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i) Create a web page to show the the booked ground details and a button to change the slot request.                                                                   ii) Create a business logic so that if coach will click on change request button coach needs to select a specific new slot from dropdown (hidden unless the change button is clicked on).  </t>
+  </si>
+  <si>
+    <t>Acceptance Criteria - Successfully able to raise the change request.</t>
+  </si>
+  <si>
+    <t>Create business logic so that after booking/cancelling/change in slot sms will be sent to the respective person</t>
+  </si>
+  <si>
+    <t>Scrum Role</t>
+  </si>
+  <si>
+    <t>Rashi- Scrum Master</t>
+  </si>
+  <si>
+    <t>Ashish - Product Owner</t>
+  </si>
+  <si>
+    <t>Ritu - Dev</t>
+  </si>
+  <si>
+    <t>Sandya - QA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,8 +462,15 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,6 +501,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -605,10 +644,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -679,8 +719,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="40% - Accent4" xfId="1" builtinId="43"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -992,14 +1036,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" customWidth="1"/>
@@ -1007,13 +1051,13 @@
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1021,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1029,7 +1073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1037,7 +1081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="39.75" thickBot="1">
+    <row r="5" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1045,17 +1089,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
         <v>6</v>
       </c>
@@ -1066,7 +1110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1077,7 +1121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1088,7 +1132,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
@@ -1099,7 +1143,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1115,9 +1159,9 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C11" r:id="rId3" xr:uid="{066A3887-A212-41B0-A7CF-498DF015C610}"/>
+    <hyperlink ref="C13" r:id="rId1"/>
+    <hyperlink ref="C14" r:id="rId2"/>
+    <hyperlink ref="C11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -1125,142 +1169,170 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="30">
+    <row r="21" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="30">
+    <row r="23" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="20" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="20" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1271,14 +1343,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="35.140625" customWidth="1"/>
@@ -1287,7 +1359,7 @@
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>45</v>
       </c>
@@ -1304,7 +1376,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135">
+    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>50</v>
       </c>
@@ -1312,153 +1384,163 @@
         <v>51</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="25" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="150">
-      <c r="B3" s="28" t="s">
+      <c r="C3" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D4" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="69.75" customHeight="1">
-      <c r="B4" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C5" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="26" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="B6" s="26" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="67.5" customHeight="1">
-      <c r="B5" s="21"/>
-      <c r="C5" s="26"/>
-    </row>
-    <row r="6" spans="1:5" ht="180">
-      <c r="A6" s="21" t="s">
+      <c r="C6" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="26" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="C7" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="25" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="210">
-      <c r="B7" s="26" t="s">
+      <c r="D8" s="22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="B9" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="C9" s="22" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="225">
-      <c r="C8" s="22" t="s">
+      <c r="D9" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="22"/>
+    </row>
+    <row r="11" spans="1:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="B11" s="26" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="45">
-      <c r="B9" s="25" t="s">
+      <c r="C11" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="D11" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="B12" s="26" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="150">
-      <c r="A10" s="29" t="s">
+      <c r="C12" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="D12" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="B13" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="C13" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="C11" s="22"/>
-    </row>
-    <row r="12" spans="1:5" ht="108" customHeight="1">
-      <c r="A12" s="21" t="s">
+      <c r="B15" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="147" customHeight="1">
-      <c r="A13" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="130.5" customHeight="1">
-      <c r="A14" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="26" t="s">
+      <c r="D15" s="26" t="s">
         <v>85</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45">
-      <c r="A15" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates PPT and benefits
</commit_message>
<xml_diff>
--- a/Agile-ASSIGNMENT.xlsx
+++ b/Agile-ASSIGNMENT.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BITS_Agile_Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tcsdatacifs09.corp.trizetto.com\citrixprofiles\sandya.shanmugham.upm\DATA\Documents\Agile Assignment\BITS_Agile_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Evalution citeria " sheetId="1" r:id="rId1"/>
     <sheet name="Case Study 1  Facify-me" sheetId="2" r:id="rId2"/>
-    <sheet name="Case Study 1 - User Stories" sheetId="3" r:id="rId3"/>
+    <sheet name="Facify-me_BacklogUserstories" sheetId="3" r:id="rId3"/>
+    <sheet name="Facify-me_Agile_Ceremonies" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t xml:space="preserve">Assignment evalution citeria </t>
   </si>
@@ -388,12 +389,80 @@
   <si>
     <t>8. SMS functionality</t>
   </si>
+  <si>
+    <t>Sprint Planning</t>
+  </si>
+  <si>
+    <t>Daily Stand-Up</t>
+  </si>
+  <si>
+    <t>Sprint Review</t>
+  </si>
+  <si>
+    <t>Sprint Retrospective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backlog Grooming </t>
+  </si>
+  <si>
+    <t>Sl.No</t>
+  </si>
+  <si>
+    <t>Ceremonies</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last for around 15 minutes of regular daily short meetings </t>
+  </si>
+  <si>
+    <t xml:space="preserve">These usually last for two hours as per each week that will go into the sprint or
+First day of sprint /last day of previous sprint </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> »Essential preceding ritual of every sprint
+ »Ensures items are  transferred from the product backlog to the sprint backlog, ensuring they are ready to commit to the completion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">»Team members discuss any obstruction in their work process and also report on their daily progress.
+»Extremely helpful to keep the team members encouraged on the path of success and improvement. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">»Product owner  helps the Scrum team with prioritizing the order of the product backlog. 
+»Members identify what needs to be added as well as root out defective or outdated items which need to be eliminated from the list. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doesn’t really have to be  fixed schedule or frequency 
+Product owners call's to fix the frequency of shedule </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> » Scrum team demonstrates the work done to the PO and the stakeholders present 
+ »  Feedback and relevant new business context is discussed upon, and finally the updating of the product backlog according to how the discussion proceeds.
+</t>
+  </si>
+  <si>
+    <t>Towards the end of the sprint ,usually last for around two hours or lesser depends on  sprints size.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">» Identifies the opportunities and finally creating a plan as to how certain improvements can be brought upon in the upcoming sprint. 
+» Discusses  stronger points of the sprint and continue to apply them in upcoming sprints  
+»  Team members try to work on their efficiency of work and their delivered quality. 
+</t>
+  </si>
+  <si>
+    <t>Usually last for 45 minutes as per each week that went into the sprint or end of the sprint</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,6 +538,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -508,7 +591,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -643,12 +726,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -716,6 +895,42 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -727,7 +942,157 @@
     <cellStyle name="40% - Accent4" xfId="1" builtinId="43"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -738,6 +1103,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E9" totalsRowShown="0">
+  <autoFilter ref="A1:E9"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Module"/>
+    <tableColumn id="2" name="Details" dataDxfId="9"/>
+    <tableColumn id="3" name="User  Stories" dataDxfId="8"/>
+    <tableColumn id="4" name="Acceptance Criteria"/>
+    <tableColumn id="5" name="Story point "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D6" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D6"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Sl.No" dataDxfId="3"/>
+    <tableColumn id="2" name="Ceremonies" dataDxfId="2"/>
+    <tableColumn id="3" name="Benefits" dataDxfId="1"/>
+    <tableColumn id="4" name="Schedule" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1039,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,10 +1444,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="44"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -1172,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection sqref="A1:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,5 +1938,116 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="51.5703125" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="31">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
+        <v>3</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>4</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
+        <v>5</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>